<commit_message>
test: fix expressions in api test data
</commit_message>
<xml_diff>
--- a/molgenis-api-tests/src/test/resources/RestControllerV1_API_TestEMX.xlsx
+++ b/molgenis-api-tests/src/test/resources/RestControllerV1_API_TestEMX.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-api-tests/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DA709C-B1D3-E54B-9E98-DABD91733DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="0" windowWidth="33860" windowHeight="18480" activeTab="5"/>
+    <workbookView xWindow="33300" yWindow="-12360" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="V1_API_TypeTestRefAPIV1" sheetId="2" r:id="rId5"/>
     <sheet name="V1_API_Items" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -491,12 +497,6 @@
     <t>driverslicence</t>
   </si>
   <si>
-    <t>$('age').ge(18).value()</t>
-  </si>
-  <si>
-    <t>$('driverslicence').isNull().not().or($('age').isNull()).or($('age').lt(18)).value()</t>
-  </si>
-  <si>
     <t>defaultValue</t>
   </si>
   <si>
@@ -840,12 +840,18 @@
   </si>
   <si>
     <t>Items</t>
+  </si>
+  <si>
+    <t>{age} &gt;= 18</t>
+  </si>
+  <si>
+    <t>{driverslicence} notempty or {age} empty or {age} &lt; 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1047,6 +1053,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1338,20 +1347,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1362,20 +1371,20 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" t="s">
         <v>259</v>
       </c>
-      <c r="C2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1389,14 +1398,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -1404,7 +1413,7 @@
     <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1421,74 +1430,74 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>262</v>
       </c>
-      <c r="B2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="s">
         <v>262</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>263</v>
       </c>
-      <c r="B3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" t="s">
         <v>263</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C5" t="s">
-        <v>265</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>271</v>
-      </c>
-      <c r="B6" t="s">
-        <v>260</v>
-      </c>
       <c r="C6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1503,14 +1512,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView topLeftCell="J23" workbookViewId="0">
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5" customWidth="1"/>
@@ -1520,13 +1529,13 @@
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1549,7 +1558,7 @@
         <v>76</v>
       </c>
       <c r="H1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s">
         <v>79</v>
@@ -1567,7 +1576,7 @@
         <v>89</v>
       </c>
       <c r="N1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O1" t="s">
         <v>90</v>
@@ -1591,12 +1600,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
@@ -1611,18 +1620,18 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
@@ -1640,18 +1649,18 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1666,15 +1675,15 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -1692,15 +1701,15 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -1718,18 +1727,18 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="U6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
         <v>143</v>
@@ -1741,18 +1750,18 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="U7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -1773,15 +1782,15 @@
         <v>142</v>
       </c>
       <c r="U8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C9" t="s">
         <v>63</v>
@@ -1802,24 +1811,24 @@
         <v>142</v>
       </c>
       <c r="T9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="U9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1831,24 +1840,24 @@
         <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="U10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C11" t="s">
         <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1860,21 +1869,21 @@
         <v>3</v>
       </c>
       <c r="T11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C12" t="s">
         <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1883,27 +1892,27 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C13" t="s">
         <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1912,18 +1921,18 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C14" t="s">
         <v>67</v>
@@ -1941,18 +1950,18 @@
         <v>1</v>
       </c>
       <c r="T14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="U14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
         <v>67</v>
@@ -1967,18 +1976,18 @@
         <v>42095</v>
       </c>
       <c r="T15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>68</v>
@@ -1993,15 +2002,15 @@
         <v>6</v>
       </c>
       <c r="U16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
@@ -2019,18 +2028,18 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="U17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C18" t="s">
         <v>69</v>
@@ -2048,18 +2057,18 @@
         <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U18" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
         <v>69</v>
@@ -2074,18 +2083,18 @@
         <v>15.666</v>
       </c>
       <c r="T19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U19" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
         <v>70</v>
@@ -2097,24 +2106,24 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
       </c>
       <c r="T20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="U20" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C21" t="s">
         <v>70</v>
@@ -2129,18 +2138,18 @@
         <v>7</v>
       </c>
       <c r="T21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C22" t="s">
         <v>77</v>
@@ -2161,15 +2170,15 @@
         <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C23" t="s">
         <v>77</v>
@@ -2187,18 +2196,18 @@
         <v>10</v>
       </c>
       <c r="T23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="U23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
         <v>71</v>
@@ -2213,15 +2222,15 @@
         <v>11</v>
       </c>
       <c r="U24" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C25" t="s">
         <v>71</v>
@@ -2233,24 +2242,24 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="U25" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C26" t="s">
         <v>72</v>
@@ -2262,24 +2271,24 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N26" t="b">
         <v>1</v>
       </c>
       <c r="T26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="U26" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C27" t="s">
         <v>72</v>
@@ -2291,21 +2300,21 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="T27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="U27" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C28" t="s">
         <v>64</v>
@@ -2323,18 +2332,18 @@
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="U28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C29" t="s">
         <v>64</v>
@@ -2349,15 +2358,15 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C30" t="s">
         <v>64</v>
@@ -2375,18 +2384,18 @@
         <v>10</v>
       </c>
       <c r="T30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="U30" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C31" t="s">
         <v>64</v>
@@ -2404,18 +2413,18 @@
         <v>0</v>
       </c>
       <c r="T31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C32" t="s">
         <v>73</v>
@@ -2430,18 +2439,18 @@
         <v>12342151234</v>
       </c>
       <c r="T32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="U32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
         <v>73</v>
@@ -2456,15 +2465,15 @@
         <v>12342151234</v>
       </c>
       <c r="U33" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C34" t="s">
         <v>73</v>
@@ -2488,18 +2497,18 @@
         <v>1</v>
       </c>
       <c r="T34" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="U34" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C35" t="s">
         <v>73</v>
@@ -2523,24 +2532,24 @@
         <v>1</v>
       </c>
       <c r="T35" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="U35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -2552,21 +2561,21 @@
         <v>1</v>
       </c>
       <c r="T36" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C37" t="s">
         <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -2575,12 +2584,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C38" t="s">
         <v>63</v>
@@ -2598,18 +2607,18 @@
         <v>1</v>
       </c>
       <c r="T38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="U38" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C39" t="s">
         <v>63</v>
@@ -2624,18 +2633,18 @@
         <v>39</v>
       </c>
       <c r="T39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="U39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -2650,15 +2659,15 @@
         <v>40</v>
       </c>
       <c r="U40" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -2673,24 +2682,24 @@
         <v>41</v>
       </c>
       <c r="T41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="U41" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C42" t="s">
         <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -2702,21 +2711,21 @@
         <v>1</v>
       </c>
       <c r="T42" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C43" t="s">
         <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -2725,15 +2734,15 @@
         <v>1</v>
       </c>
       <c r="T43" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C44" t="s">
         <v>63</v>
@@ -2751,18 +2760,18 @@
         <v>0</v>
       </c>
       <c r="T44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U44" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C45" t="s">
         <v>63</v>
@@ -2774,24 +2783,24 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O45" t="b">
         <v>0</v>
       </c>
       <c r="T45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="U45" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C46" t="s">
         <v>63</v>
@@ -2806,15 +2815,15 @@
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C47" t="s">
         <v>64</v>
@@ -2829,24 +2838,24 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="U47" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>132</v>
       </c>
       <c r="B48" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C48" t="s">
         <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -2858,18 +2867,18 @@
         <v>1</v>
       </c>
       <c r="T48" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B49" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C49" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -2878,18 +2887,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C50" t="s">
         <v>75</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -2904,18 +2913,18 @@
         <v>139</v>
       </c>
       <c r="T50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="U50" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C51" t="s">
         <v>64</v>
@@ -2933,18 +2942,18 @@
         <v>29</v>
       </c>
       <c r="T51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="U51" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>63</v>
@@ -2968,15 +2977,15 @@
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="U52" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>64</v>
@@ -3003,18 +3012,18 @@
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="U53" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C54" t="s">
         <v>63</v>
@@ -3026,18 +3035,18 @@
         <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="U54" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>152</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C55" t="s">
         <v>64</v>
@@ -3049,18 +3058,18 @@
         <v>1</v>
       </c>
       <c r="T55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="U55" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>154</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C56" t="s">
         <v>65</v>
@@ -3072,24 +3081,24 @@
         <v>1</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="S56" t="s">
-        <v>156</v>
+        <v>271</v>
       </c>
       <c r="T56" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="U56" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C57" t="s">
         <v>63</v>
@@ -3104,18 +3113,18 @@
         <v>1</v>
       </c>
       <c r="T57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U57" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C58" t="s">
         <v>63</v>
@@ -3133,10 +3142,10 @@
         <v>1</v>
       </c>
       <c r="T58" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U58" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3151,14 +3160,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
@@ -3188,7 +3197,7 @@
     <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -3322,10 +3331,10 @@
         <v>132</v>
       </c>
       <c r="AS1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3459,7 +3468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3593,7 +3602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3673,7 +3682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3807,7 +3816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3941,7 +3950,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4018,7 +4027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4149,7 +4158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4280,7 +4289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4357,7 +4366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4488,7 +4497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4619,7 +4628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4696,7 +4705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4827,7 +4836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4958,7 +4967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5035,7 +5044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5112,7 +5121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5243,7 +5252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5374,7 +5383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5451,7 +5460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5582,7 +5591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5710,7 +5719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5784,7 +5793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5912,7 +5921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6040,7 +6049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6114,7 +6123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6242,7 +6251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6370,7 +6379,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6444,7 +6453,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6572,7 +6581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6700,7 +6709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6774,7 +6783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6902,7 +6911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -7030,7 +7039,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -7104,7 +7113,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -7178,7 +7187,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -7306,7 +7315,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7434,7 +7443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7510,130 +7519,130 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="P3" r:id="rId2"/>
-    <hyperlink ref="Q2" r:id="rId3"/>
-    <hyperlink ref="P4" r:id="rId4"/>
-    <hyperlink ref="Q3" r:id="rId5"/>
-    <hyperlink ref="V2" r:id="rId6"/>
-    <hyperlink ref="V3" r:id="rId7"/>
-    <hyperlink ref="V4" r:id="rId8"/>
-    <hyperlink ref="W2" r:id="rId9"/>
-    <hyperlink ref="W3" r:id="rId10"/>
-    <hyperlink ref="P5" r:id="rId11"/>
-    <hyperlink ref="P6" r:id="rId12"/>
-    <hyperlink ref="Q5" r:id="rId13"/>
-    <hyperlink ref="P7" r:id="rId14"/>
-    <hyperlink ref="Q6" r:id="rId15"/>
-    <hyperlink ref="V5" r:id="rId16"/>
-    <hyperlink ref="V6" r:id="rId17"/>
-    <hyperlink ref="V7" r:id="rId18"/>
-    <hyperlink ref="W5" r:id="rId19"/>
-    <hyperlink ref="W6" r:id="rId20"/>
-    <hyperlink ref="P8" r:id="rId21"/>
-    <hyperlink ref="P9" r:id="rId22"/>
-    <hyperlink ref="Q8" r:id="rId23"/>
-    <hyperlink ref="P10" r:id="rId24"/>
-    <hyperlink ref="Q9" r:id="rId25"/>
-    <hyperlink ref="V8" r:id="rId26"/>
-    <hyperlink ref="V9" r:id="rId27"/>
-    <hyperlink ref="V10" r:id="rId28"/>
-    <hyperlink ref="W8" r:id="rId29"/>
-    <hyperlink ref="W9" r:id="rId30"/>
-    <hyperlink ref="P11" r:id="rId31"/>
-    <hyperlink ref="P12" r:id="rId32"/>
-    <hyperlink ref="Q11" r:id="rId33"/>
-    <hyperlink ref="P13" r:id="rId34"/>
-    <hyperlink ref="Q12" r:id="rId35"/>
-    <hyperlink ref="V11" r:id="rId36"/>
-    <hyperlink ref="V12" r:id="rId37"/>
-    <hyperlink ref="V13" r:id="rId38"/>
-    <hyperlink ref="W11" r:id="rId39"/>
-    <hyperlink ref="W12" r:id="rId40"/>
-    <hyperlink ref="P14" r:id="rId41"/>
-    <hyperlink ref="P15" r:id="rId42"/>
-    <hyperlink ref="Q14" r:id="rId43"/>
-    <hyperlink ref="P16" r:id="rId44"/>
-    <hyperlink ref="Q15" r:id="rId45"/>
-    <hyperlink ref="V14" r:id="rId46"/>
-    <hyperlink ref="V15" r:id="rId47"/>
-    <hyperlink ref="V16" r:id="rId48"/>
-    <hyperlink ref="W14" r:id="rId49"/>
-    <hyperlink ref="W15" r:id="rId50"/>
-    <hyperlink ref="P17" r:id="rId51"/>
-    <hyperlink ref="V17" r:id="rId52"/>
-    <hyperlink ref="P18" r:id="rId53"/>
-    <hyperlink ref="P19" r:id="rId54"/>
-    <hyperlink ref="Q18" r:id="rId55"/>
-    <hyperlink ref="P20" r:id="rId56"/>
-    <hyperlink ref="Q19" r:id="rId57"/>
-    <hyperlink ref="V18" r:id="rId58"/>
-    <hyperlink ref="V19" r:id="rId59"/>
-    <hyperlink ref="V20" r:id="rId60"/>
-    <hyperlink ref="W18" r:id="rId61"/>
-    <hyperlink ref="W19" r:id="rId62"/>
-    <hyperlink ref="P21" r:id="rId63"/>
-    <hyperlink ref="P22" r:id="rId64"/>
-    <hyperlink ref="Q21" r:id="rId65"/>
-    <hyperlink ref="P23" r:id="rId66"/>
-    <hyperlink ref="Q22" r:id="rId67"/>
-    <hyperlink ref="V21" r:id="rId68"/>
-    <hyperlink ref="V22" r:id="rId69"/>
-    <hyperlink ref="V23" r:id="rId70"/>
-    <hyperlink ref="W21" r:id="rId71"/>
-    <hyperlink ref="W22" r:id="rId72"/>
-    <hyperlink ref="P24" r:id="rId73"/>
-    <hyperlink ref="P25" r:id="rId74"/>
-    <hyperlink ref="Q24" r:id="rId75"/>
-    <hyperlink ref="P26" r:id="rId76"/>
-    <hyperlink ref="Q25" r:id="rId77"/>
-    <hyperlink ref="V24" r:id="rId78"/>
-    <hyperlink ref="V25" r:id="rId79"/>
-    <hyperlink ref="V26" r:id="rId80"/>
-    <hyperlink ref="W24" r:id="rId81"/>
-    <hyperlink ref="W25" r:id="rId82"/>
-    <hyperlink ref="P27" r:id="rId83"/>
-    <hyperlink ref="P28" r:id="rId84"/>
-    <hyperlink ref="Q27" r:id="rId85"/>
-    <hyperlink ref="P29" r:id="rId86"/>
-    <hyperlink ref="Q28" r:id="rId87"/>
-    <hyperlink ref="V27" r:id="rId88"/>
-    <hyperlink ref="V28" r:id="rId89"/>
-    <hyperlink ref="V29" r:id="rId90"/>
-    <hyperlink ref="W27" r:id="rId91"/>
-    <hyperlink ref="W28" r:id="rId92"/>
-    <hyperlink ref="P30" r:id="rId93"/>
-    <hyperlink ref="P31" r:id="rId94"/>
-    <hyperlink ref="Q30" r:id="rId95"/>
-    <hyperlink ref="P32" r:id="rId96"/>
-    <hyperlink ref="Q31" r:id="rId97"/>
-    <hyperlink ref="V30" r:id="rId98"/>
-    <hyperlink ref="V31" r:id="rId99"/>
-    <hyperlink ref="V32" r:id="rId100"/>
-    <hyperlink ref="W30" r:id="rId101"/>
-    <hyperlink ref="W31" r:id="rId102"/>
-    <hyperlink ref="P33" r:id="rId103"/>
-    <hyperlink ref="P34" r:id="rId104"/>
-    <hyperlink ref="Q33" r:id="rId105"/>
-    <hyperlink ref="P35" r:id="rId106"/>
-    <hyperlink ref="Q34" r:id="rId107"/>
-    <hyperlink ref="V33" r:id="rId108"/>
-    <hyperlink ref="V34" r:id="rId109"/>
-    <hyperlink ref="V35" r:id="rId110"/>
-    <hyperlink ref="W33" r:id="rId111"/>
-    <hyperlink ref="W34" r:id="rId112"/>
-    <hyperlink ref="P36" r:id="rId113"/>
-    <hyperlink ref="V36" r:id="rId114"/>
-    <hyperlink ref="P37" r:id="rId115"/>
-    <hyperlink ref="P38" r:id="rId116"/>
-    <hyperlink ref="Q37" r:id="rId117"/>
-    <hyperlink ref="P39" r:id="rId118"/>
-    <hyperlink ref="Q38" r:id="rId119"/>
-    <hyperlink ref="V37" r:id="rId120"/>
-    <hyperlink ref="V38" r:id="rId121"/>
-    <hyperlink ref="V39" r:id="rId122"/>
-    <hyperlink ref="W37" r:id="rId123"/>
-    <hyperlink ref="W38" r:id="rId124"/>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="Q2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="P4" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="Q3" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="V2" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="V3" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="V4" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="W2" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="W3" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="P5" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="P6" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="Q5" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="P7" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="Q6" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="V5" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="V6" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="V7" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="W5" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="W6" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="P8" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="P9" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="Q8" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
+    <hyperlink ref="P10" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
+    <hyperlink ref="Q9" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
+    <hyperlink ref="V8" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
+    <hyperlink ref="V9" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
+    <hyperlink ref="V10" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
+    <hyperlink ref="W8" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
+    <hyperlink ref="W9" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
+    <hyperlink ref="P11" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
+    <hyperlink ref="P12" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
+    <hyperlink ref="Q11" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
+    <hyperlink ref="P13" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
+    <hyperlink ref="Q12" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
+    <hyperlink ref="V11" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
+    <hyperlink ref="V12" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
+    <hyperlink ref="V13" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
+    <hyperlink ref="W11" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
+    <hyperlink ref="W12" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
+    <hyperlink ref="P14" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
+    <hyperlink ref="P15" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
+    <hyperlink ref="Q14" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
+    <hyperlink ref="P16" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
+    <hyperlink ref="Q15" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
+    <hyperlink ref="V14" r:id="rId46" xr:uid="{00000000-0004-0000-0300-00002D000000}"/>
+    <hyperlink ref="V15" r:id="rId47" xr:uid="{00000000-0004-0000-0300-00002E000000}"/>
+    <hyperlink ref="V16" r:id="rId48" xr:uid="{00000000-0004-0000-0300-00002F000000}"/>
+    <hyperlink ref="W14" r:id="rId49" xr:uid="{00000000-0004-0000-0300-000030000000}"/>
+    <hyperlink ref="W15" r:id="rId50" xr:uid="{00000000-0004-0000-0300-000031000000}"/>
+    <hyperlink ref="P17" r:id="rId51" xr:uid="{00000000-0004-0000-0300-000032000000}"/>
+    <hyperlink ref="V17" r:id="rId52" xr:uid="{00000000-0004-0000-0300-000033000000}"/>
+    <hyperlink ref="P18" r:id="rId53" xr:uid="{00000000-0004-0000-0300-000034000000}"/>
+    <hyperlink ref="P19" r:id="rId54" xr:uid="{00000000-0004-0000-0300-000035000000}"/>
+    <hyperlink ref="Q18" r:id="rId55" xr:uid="{00000000-0004-0000-0300-000036000000}"/>
+    <hyperlink ref="P20" r:id="rId56" xr:uid="{00000000-0004-0000-0300-000037000000}"/>
+    <hyperlink ref="Q19" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000038000000}"/>
+    <hyperlink ref="V18" r:id="rId58" xr:uid="{00000000-0004-0000-0300-000039000000}"/>
+    <hyperlink ref="V19" r:id="rId59" xr:uid="{00000000-0004-0000-0300-00003A000000}"/>
+    <hyperlink ref="V20" r:id="rId60" xr:uid="{00000000-0004-0000-0300-00003B000000}"/>
+    <hyperlink ref="W18" r:id="rId61" xr:uid="{00000000-0004-0000-0300-00003C000000}"/>
+    <hyperlink ref="W19" r:id="rId62" xr:uid="{00000000-0004-0000-0300-00003D000000}"/>
+    <hyperlink ref="P21" r:id="rId63" xr:uid="{00000000-0004-0000-0300-00003E000000}"/>
+    <hyperlink ref="P22" r:id="rId64" xr:uid="{00000000-0004-0000-0300-00003F000000}"/>
+    <hyperlink ref="Q21" r:id="rId65" xr:uid="{00000000-0004-0000-0300-000040000000}"/>
+    <hyperlink ref="P23" r:id="rId66" xr:uid="{00000000-0004-0000-0300-000041000000}"/>
+    <hyperlink ref="Q22" r:id="rId67" xr:uid="{00000000-0004-0000-0300-000042000000}"/>
+    <hyperlink ref="V21" r:id="rId68" xr:uid="{00000000-0004-0000-0300-000043000000}"/>
+    <hyperlink ref="V22" r:id="rId69" xr:uid="{00000000-0004-0000-0300-000044000000}"/>
+    <hyperlink ref="V23" r:id="rId70" xr:uid="{00000000-0004-0000-0300-000045000000}"/>
+    <hyperlink ref="W21" r:id="rId71" xr:uid="{00000000-0004-0000-0300-000046000000}"/>
+    <hyperlink ref="W22" r:id="rId72" xr:uid="{00000000-0004-0000-0300-000047000000}"/>
+    <hyperlink ref="P24" r:id="rId73" xr:uid="{00000000-0004-0000-0300-000048000000}"/>
+    <hyperlink ref="P25" r:id="rId74" xr:uid="{00000000-0004-0000-0300-000049000000}"/>
+    <hyperlink ref="Q24" r:id="rId75" xr:uid="{00000000-0004-0000-0300-00004A000000}"/>
+    <hyperlink ref="P26" r:id="rId76" xr:uid="{00000000-0004-0000-0300-00004B000000}"/>
+    <hyperlink ref="Q25" r:id="rId77" xr:uid="{00000000-0004-0000-0300-00004C000000}"/>
+    <hyperlink ref="V24" r:id="rId78" xr:uid="{00000000-0004-0000-0300-00004D000000}"/>
+    <hyperlink ref="V25" r:id="rId79" xr:uid="{00000000-0004-0000-0300-00004E000000}"/>
+    <hyperlink ref="V26" r:id="rId80" xr:uid="{00000000-0004-0000-0300-00004F000000}"/>
+    <hyperlink ref="W24" r:id="rId81" xr:uid="{00000000-0004-0000-0300-000050000000}"/>
+    <hyperlink ref="W25" r:id="rId82" xr:uid="{00000000-0004-0000-0300-000051000000}"/>
+    <hyperlink ref="P27" r:id="rId83" xr:uid="{00000000-0004-0000-0300-000052000000}"/>
+    <hyperlink ref="P28" r:id="rId84" xr:uid="{00000000-0004-0000-0300-000053000000}"/>
+    <hyperlink ref="Q27" r:id="rId85" xr:uid="{00000000-0004-0000-0300-000054000000}"/>
+    <hyperlink ref="P29" r:id="rId86" xr:uid="{00000000-0004-0000-0300-000055000000}"/>
+    <hyperlink ref="Q28" r:id="rId87" xr:uid="{00000000-0004-0000-0300-000056000000}"/>
+    <hyperlink ref="V27" r:id="rId88" xr:uid="{00000000-0004-0000-0300-000057000000}"/>
+    <hyperlink ref="V28" r:id="rId89" xr:uid="{00000000-0004-0000-0300-000058000000}"/>
+    <hyperlink ref="V29" r:id="rId90" xr:uid="{00000000-0004-0000-0300-000059000000}"/>
+    <hyperlink ref="W27" r:id="rId91" xr:uid="{00000000-0004-0000-0300-00005A000000}"/>
+    <hyperlink ref="W28" r:id="rId92" xr:uid="{00000000-0004-0000-0300-00005B000000}"/>
+    <hyperlink ref="P30" r:id="rId93" xr:uid="{00000000-0004-0000-0300-00005C000000}"/>
+    <hyperlink ref="P31" r:id="rId94" xr:uid="{00000000-0004-0000-0300-00005D000000}"/>
+    <hyperlink ref="Q30" r:id="rId95" xr:uid="{00000000-0004-0000-0300-00005E000000}"/>
+    <hyperlink ref="P32" r:id="rId96" xr:uid="{00000000-0004-0000-0300-00005F000000}"/>
+    <hyperlink ref="Q31" r:id="rId97" xr:uid="{00000000-0004-0000-0300-000060000000}"/>
+    <hyperlink ref="V30" r:id="rId98" xr:uid="{00000000-0004-0000-0300-000061000000}"/>
+    <hyperlink ref="V31" r:id="rId99" xr:uid="{00000000-0004-0000-0300-000062000000}"/>
+    <hyperlink ref="V32" r:id="rId100" xr:uid="{00000000-0004-0000-0300-000063000000}"/>
+    <hyperlink ref="W30" r:id="rId101" xr:uid="{00000000-0004-0000-0300-000064000000}"/>
+    <hyperlink ref="W31" r:id="rId102" xr:uid="{00000000-0004-0000-0300-000065000000}"/>
+    <hyperlink ref="P33" r:id="rId103" xr:uid="{00000000-0004-0000-0300-000066000000}"/>
+    <hyperlink ref="P34" r:id="rId104" xr:uid="{00000000-0004-0000-0300-000067000000}"/>
+    <hyperlink ref="Q33" r:id="rId105" xr:uid="{00000000-0004-0000-0300-000068000000}"/>
+    <hyperlink ref="P35" r:id="rId106" xr:uid="{00000000-0004-0000-0300-000069000000}"/>
+    <hyperlink ref="Q34" r:id="rId107" xr:uid="{00000000-0004-0000-0300-00006A000000}"/>
+    <hyperlink ref="V33" r:id="rId108" xr:uid="{00000000-0004-0000-0300-00006B000000}"/>
+    <hyperlink ref="V34" r:id="rId109" xr:uid="{00000000-0004-0000-0300-00006C000000}"/>
+    <hyperlink ref="V35" r:id="rId110" xr:uid="{00000000-0004-0000-0300-00006D000000}"/>
+    <hyperlink ref="W33" r:id="rId111" xr:uid="{00000000-0004-0000-0300-00006E000000}"/>
+    <hyperlink ref="W34" r:id="rId112" xr:uid="{00000000-0004-0000-0300-00006F000000}"/>
+    <hyperlink ref="P36" r:id="rId113" xr:uid="{00000000-0004-0000-0300-000070000000}"/>
+    <hyperlink ref="V36" r:id="rId114" xr:uid="{00000000-0004-0000-0300-000071000000}"/>
+    <hyperlink ref="P37" r:id="rId115" xr:uid="{00000000-0004-0000-0300-000072000000}"/>
+    <hyperlink ref="P38" r:id="rId116" xr:uid="{00000000-0004-0000-0300-000073000000}"/>
+    <hyperlink ref="Q37" r:id="rId117" xr:uid="{00000000-0004-0000-0300-000074000000}"/>
+    <hyperlink ref="P39" r:id="rId118" xr:uid="{00000000-0004-0000-0300-000075000000}"/>
+    <hyperlink ref="Q38" r:id="rId119" xr:uid="{00000000-0004-0000-0300-000076000000}"/>
+    <hyperlink ref="V37" r:id="rId120" xr:uid="{00000000-0004-0000-0300-000077000000}"/>
+    <hyperlink ref="V38" r:id="rId121" xr:uid="{00000000-0004-0000-0300-000078000000}"/>
+    <hyperlink ref="V39" r:id="rId122" xr:uid="{00000000-0004-0000-0300-000079000000}"/>
+    <hyperlink ref="W37" r:id="rId123" xr:uid="{00000000-0004-0000-0300-00007A000000}"/>
+    <hyperlink ref="W38" r:id="rId124" xr:uid="{00000000-0004-0000-0300-00007B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7645,16 +7654,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7662,7 +7671,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7670,7 +7679,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7678,7 +7687,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7686,7 +7695,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -7694,7 +7703,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -7713,16 +7722,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7730,7 +7739,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7738,7 +7747,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7746,7 +7755,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7754,7 +7763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -7762,7 +7771,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
test: update test files
</commit_message>
<xml_diff>
--- a/molgenis-api-tests/src/test/resources/RestControllerV1_API_TestEMX.xlsx
+++ b/molgenis-api-tests/src/test/resources/RestControllerV1_API_TestEMX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-api-tests/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DA709C-B1D3-E54B-9E98-DABD91733DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D470515-549A-9343-B8E1-778E37C0F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33300" yWindow="-12360" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33300" yWindow="-12360" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
@@ -842,10 +842,10 @@
     <t>Items</t>
   </si>
   <si>
-    <t>{age} &gt;= 18</t>
-  </si>
-  <si>
     <t>{driverslicence} notempty or {age} empty or {age} &lt; 18</t>
+  </si>
+  <si>
+    <t>{age} notempty &amp;&amp; {age} &gt;= 18</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="J23" workbookViewId="0">
-      <selection activeCell="S56" sqref="S56"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1529,7 +1529,7 @@
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
@@ -3081,10 +3081,10 @@
         <v>1</v>
       </c>
       <c r="O56" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S56" t="s">
         <v>270</v>
-      </c>
-      <c r="S56" t="s">
-        <v>271</v>
       </c>
       <c r="T56" t="s">
         <v>206</v>

</xml_diff>

<commit_message>
[FEAT] visible expression overrides nullable expression (#9260)
* feat: nullableExpression is true if visibleExpression is false

* fix: update system metadata nullableExpression for attributes with a visibleExpression

* test: update test files
</commit_message>
<xml_diff>
--- a/molgenis-api-tests/src/test/resources/RestControllerV1_API_TestEMX.xlsx
+++ b/molgenis-api-tests/src/test/resources/RestControllerV1_API_TestEMX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-api-tests/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DA709C-B1D3-E54B-9E98-DABD91733DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D470515-549A-9343-B8E1-778E37C0F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33300" yWindow="-12360" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33300" yWindow="-12360" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
@@ -842,10 +842,10 @@
     <t>Items</t>
   </si>
   <si>
-    <t>{age} &gt;= 18</t>
-  </si>
-  <si>
     <t>{driverslicence} notempty or {age} empty or {age} &lt; 18</t>
+  </si>
+  <si>
+    <t>{age} notempty &amp;&amp; {age} &gt;= 18</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="J23" workbookViewId="0">
-      <selection activeCell="S56" sqref="S56"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1529,7 +1529,7 @@
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
@@ -3081,10 +3081,10 @@
         <v>1</v>
       </c>
       <c r="O56" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S56" t="s">
         <v>270</v>
-      </c>
-      <c r="S56" t="s">
-        <v>271</v>
       </c>
       <c r="T56" t="s">
         <v>206</v>

</xml_diff>